<commit_message>
Test Documents are  updated
</commit_message>
<xml_diff>
--- a/Test Documents/TestCases-OpenCart.xlsx
+++ b/Test Documents/TestCases-OpenCart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a3e22fe4f38f8cd/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\IdeaProjects\OpenCart\Test Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="448" documentId="8_{E92EADF8-A308-491F-AD47-BA9E21D07BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC3D41EC-70A8-4623-A22F-B71CA134E662}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9D61E9-660B-485F-A9C3-BE04B83C997D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="891" firstSheet="1" activeTab="1" xr2:uid="{AB1EE694-DF79-45FE-B023-350A76CFD5F6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="891" activeTab="1" xr2:uid="{AB1EE694-DF79-45FE-B023-350A76CFD5F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Version-History" sheetId="1" r:id="rId1"/>
@@ -12672,7 +12672,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -12739,7 +12739,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="56">
-        <v>45786</v>
+        <v>45829</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="7"/>
@@ -12750,7 +12750,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="56">
-        <v>45792</v>
+        <v>45832</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="7"/>

</xml_diff>